<commit_message>
Updates to Table 1
</commit_message>
<xml_diff>
--- a/Table 1.xlsx
+++ b/Table 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\Documents\repo\finalproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ED5533-A9AF-4A86-A1D1-60A9A1D4DD62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9916FB-C4C9-4C33-A65D-B8F316B0A17D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F779DEB9-5FFF-4C92-A524-9FDA0DD5880D}"/>
+    <workbookView xWindow="4500" yWindow="1395" windowWidth="18000" windowHeight="9360" xr2:uid="{F779DEB9-5FFF-4C92-A524-9FDA0DD5880D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="184">
   <si>
     <t>Species</t>
   </si>
@@ -229,13 +229,361 @@
   </si>
   <si>
     <t>ERR2587212</t>
+  </si>
+  <si>
+    <t>SRR8710046</t>
+  </si>
+  <si>
+    <t>SRR8710047</t>
+  </si>
+  <si>
+    <t>SRR8710045</t>
+  </si>
+  <si>
+    <t>Trematomus bernacchii</t>
+  </si>
+  <si>
+    <t>SRR8710044</t>
+  </si>
+  <si>
+    <t>SRR8709999</t>
+  </si>
+  <si>
+    <t>SRR8710000</t>
+  </si>
+  <si>
+    <t>SRR8710001</t>
+  </si>
+  <si>
+    <t>SRR8710002</t>
+  </si>
+  <si>
+    <t>SRR8710003</t>
+  </si>
+  <si>
+    <t>SRR8710004</t>
+  </si>
+  <si>
+    <t>SRR8710005</t>
+  </si>
+  <si>
+    <t>SRR8710006</t>
+  </si>
+  <si>
+    <t>SRR8710007</t>
+  </si>
+  <si>
+    <t>SRR8710008</t>
+  </si>
+  <si>
+    <t>SRR8710009</t>
+  </si>
+  <si>
+    <t>SRR8710010</t>
+  </si>
+  <si>
+    <t>SRR8710011</t>
+  </si>
+  <si>
+    <t>SRR8710012</t>
+  </si>
+  <si>
+    <t>SRR8710013</t>
+  </si>
+  <si>
+    <t>SRR8710014</t>
+  </si>
+  <si>
+    <t>SRR8710015</t>
+  </si>
+  <si>
+    <t>SRR8710016</t>
+  </si>
+  <si>
+    <t>SRR8710017</t>
+  </si>
+  <si>
+    <t>SRR8710018</t>
+  </si>
+  <si>
+    <t>SRR8710019</t>
+  </si>
+  <si>
+    <t>SRR8710020</t>
+  </si>
+  <si>
+    <t>SRR8710021</t>
+  </si>
+  <si>
+    <t>SRR8710022</t>
+  </si>
+  <si>
+    <t>SRR8710023</t>
+  </si>
+  <si>
+    <t>SRR8710024</t>
+  </si>
+  <si>
+    <t>SRR8710025</t>
+  </si>
+  <si>
+    <t>SRR8710026</t>
+  </si>
+  <si>
+    <t>SRR8710027</t>
+  </si>
+  <si>
+    <t>SRR8710028</t>
+  </si>
+  <si>
+    <t>SRR8710029</t>
+  </si>
+  <si>
+    <t>SRR8710030</t>
+  </si>
+  <si>
+    <t>SRR8710031</t>
+  </si>
+  <si>
+    <t>SRR8710032</t>
+  </si>
+  <si>
+    <t>SRR8710033</t>
+  </si>
+  <si>
+    <t>SRR8710034</t>
+  </si>
+  <si>
+    <t>SRR8710035</t>
+  </si>
+  <si>
+    <t>SRR8710036</t>
+  </si>
+  <si>
+    <t>SRR8710037</t>
+  </si>
+  <si>
+    <t>SRR8710038</t>
+  </si>
+  <si>
+    <t>SRR8710039</t>
+  </si>
+  <si>
+    <t>SRR8710040</t>
+  </si>
+  <si>
+    <t>SRR8710041</t>
+  </si>
+  <si>
+    <t>SRR8710042</t>
+  </si>
+  <si>
+    <t>SRR8710043</t>
+  </si>
+  <si>
+    <t>SRR8710048</t>
+  </si>
+  <si>
+    <t>SRR8710049</t>
+  </si>
+  <si>
+    <t>gill tissue</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Dissostichus eleginoides</t>
+  </si>
+  <si>
+    <t>heart</t>
+  </si>
+  <si>
+    <t>SRR8767977</t>
+  </si>
+  <si>
+    <t>gills</t>
+  </si>
+  <si>
+    <t>SRR8767976</t>
+  </si>
+  <si>
+    <t>SRR8795863</t>
+  </si>
+  <si>
+    <t>adult male gonad</t>
+  </si>
+  <si>
+    <t>adult female gonad</t>
+  </si>
+  <si>
+    <t>SRR8795862</t>
+  </si>
+  <si>
+    <t>"morula pooled 2 days"</t>
+  </si>
+  <si>
+    <t>SRR8767973</t>
+  </si>
+  <si>
+    <t>muscle</t>
+  </si>
+  <si>
+    <t>SRR8767972</t>
+  </si>
+  <si>
+    <t>SRR8767971</t>
+  </si>
+  <si>
+    <t>liver</t>
+  </si>
+  <si>
+    <t>SRR8795689</t>
+  </si>
+  <si>
+    <t>kidney</t>
+  </si>
+  <si>
+    <t>spleen</t>
+  </si>
+  <si>
+    <t>SRR8767969</t>
+  </si>
+  <si>
+    <t>white muscle</t>
+  </si>
+  <si>
+    <t>ventricle</t>
+  </si>
+  <si>
+    <t>trunk kidney</t>
+  </si>
+  <si>
+    <t>pectoral muscle</t>
+  </si>
+  <si>
+    <t>ovary</t>
+  </si>
+  <si>
+    <t>head kidney</t>
+  </si>
+  <si>
+    <t>Sample 48_p</t>
+  </si>
+  <si>
+    <t>brain</t>
+  </si>
+  <si>
+    <t>Sample 41</t>
+  </si>
+  <si>
+    <t>blood</t>
+  </si>
+  <si>
+    <t>Sample 18</t>
+  </si>
+  <si>
+    <t>Sample 22</t>
+  </si>
+  <si>
+    <t>Sample 12_p</t>
+  </si>
+  <si>
+    <t>Sample 20_p</t>
+  </si>
+  <si>
+    <t>Sample 10_p</t>
+  </si>
+  <si>
+    <t>Sample 27_p</t>
+  </si>
+  <si>
+    <t>Sample 17_p</t>
+  </si>
+  <si>
+    <t>Sample 19_p</t>
+  </si>
+  <si>
+    <t>Sample 25_p</t>
+  </si>
+  <si>
+    <t>tesits</t>
+  </si>
+  <si>
+    <t>Sample 24_p</t>
+  </si>
+  <si>
+    <t>Sample 14_p</t>
+  </si>
+  <si>
+    <t>Sample 21_p</t>
+  </si>
+  <si>
+    <t>Sample 11_p</t>
+  </si>
+  <si>
+    <t>Sample 15_p</t>
+  </si>
+  <si>
+    <t>Sample 23_p</t>
+  </si>
+  <si>
+    <t>Sample 13_p</t>
+  </si>
+  <si>
+    <t>intestine</t>
+  </si>
+  <si>
+    <t>Sample 29_p</t>
+  </si>
+  <si>
+    <t>Sample 26_p</t>
+  </si>
+  <si>
+    <t>Sample 16_p</t>
+  </si>
+  <si>
+    <t>Sample 30</t>
+  </si>
+  <si>
+    <t>Sample 9_p</t>
+  </si>
+  <si>
+    <t>Sample 31_p</t>
+  </si>
+  <si>
+    <t>Sample 1_p</t>
+  </si>
+  <si>
+    <t>Sample 4</t>
+  </si>
+  <si>
+    <t>skin</t>
+  </si>
+  <si>
+    <t>Sample 7_p</t>
+  </si>
+  <si>
+    <t>Sample 5</t>
+  </si>
+  <si>
+    <t>Sample 6</t>
+  </si>
+  <si>
+    <t>Sample 8</t>
+  </si>
+  <si>
+    <t>Sample 3_p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +595,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,9 +627,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,506 +945,1393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CD3FE1-C10C-4CC2-9B17-9BF4EF33D9D6}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="B18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
+      <c r="B22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="D24" t="s">
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="D28" t="s">
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
-      <c r="D29" t="s">
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
-      <c r="D30" t="s">
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="D33" t="s">
+      <c r="B33" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
-      <c r="D37" t="s">
+      <c r="B37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="D38" t="s">
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="D41" t="s">
+      <c r="C41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" t="s">
+        <v>146</v>
+      </c>
+      <c r="E42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" t="s">
+        <v>145</v>
+      </c>
+      <c r="E44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
-      <c r="D47" t="s">
+      <c r="C47" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
-      <c r="D51" t="s">
+      <c r="C51" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
-      <c r="D52" t="s">
+      <c r="C52" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
-      <c r="D53" t="s">
+      <c r="C53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>39</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>39</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>39</v>
       </c>
-      <c r="D57" t="s">
+      <c r="C57" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>39</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>39</v>
       </c>
-      <c r="D59" t="s">
+      <c r="C59" t="s">
+        <v>142</v>
+      </c>
+      <c r="E59" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" t="s">
+        <v>120</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" t="s">
+        <v>120</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="C71" t="s">
+        <v>120</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" t="s">
+        <v>120</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" t="s">
+        <v>120</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" t="s">
+        <v>120</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" t="s">
+        <v>120</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" t="s">
+        <v>120</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" t="s">
+        <v>120</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" t="s">
+        <v>120</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>71</v>
+      </c>
+      <c r="C82" t="s">
+        <v>120</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" t="s">
+        <v>120</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" t="s">
+        <v>120</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C85" t="s">
+        <v>120</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" t="s">
+        <v>120</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" t="s">
+        <v>120</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>71</v>
+      </c>
+      <c r="C88" t="s">
+        <v>120</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" t="s">
+        <v>120</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" t="s">
+        <v>120</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" t="s">
+        <v>120</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" t="s">
+        <v>120</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" t="s">
+        <v>120</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" t="s">
+        <v>120</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>71</v>
+      </c>
+      <c r="C95" t="s">
+        <v>120</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>71</v>
+      </c>
+      <c r="C96" t="s">
+        <v>120</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" t="s">
+        <v>120</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>71</v>
+      </c>
+      <c r="C98" t="s">
+        <v>120</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>71</v>
+      </c>
+      <c r="C99" t="s">
+        <v>120</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>71</v>
+      </c>
+      <c r="C100" t="s">
+        <v>120</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>71</v>
+      </c>
+      <c r="C101" t="s">
+        <v>120</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>71</v>
+      </c>
+      <c r="C102" t="s">
+        <v>120</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>71</v>
+      </c>
+      <c r="C103" t="s">
+        <v>120</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>71</v>
+      </c>
+      <c r="C104" t="s">
+        <v>120</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>71</v>
+      </c>
+      <c r="C105" t="s">
+        <v>120</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>71</v>
+      </c>
+      <c r="C106" t="s">
+        <v>120</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>71</v>
+      </c>
+      <c r="C107" t="s">
+        <v>120</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>71</v>
+      </c>
+      <c r="C108" t="s">
+        <v>120</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" t="s">
+        <v>120</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>71</v>
+      </c>
+      <c r="C110" t="s">
+        <v>120</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>123</v>
+      </c>
+      <c r="C111" t="s">
+        <v>124</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C112" t="s">
+        <v>126</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113" t="s">
+        <v>129</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>123</v>
+      </c>
+      <c r="C114" t="s">
+        <v>130</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>123</v>
+      </c>
+      <c r="C115" t="s">
+        <v>132</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>123</v>
+      </c>
+      <c r="C116" t="s">
+        <v>134</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>123</v>
+      </c>
+      <c r="C117" t="s">
+        <v>137</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>123</v>
+      </c>
+      <c r="C118" t="s">
+        <v>139</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>123</v>
+      </c>
+      <c r="C119" t="s">
+        <v>140</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final READme (minus refs)
</commit_message>
<xml_diff>
--- a/Table 1.xlsx
+++ b/Table 1.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chant\Documents\repo\finalproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CF136E-9B35-4A82-A64C-C81D93AA0476}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB3CDCC-381D-4E76-A9F7-48A3B072DF00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="2085" windowWidth="18000" windowHeight="9360" xr2:uid="{F779DEB9-5FFF-4C92-A524-9FDA0DD5880D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{F779DEB9-5FFF-4C92-A524-9FDA0DD5880D}"/>
   </bookViews>
   <sheets>
     <sheet name="Transcriptomes" sheetId="1" r:id="rId1"/>
     <sheet name="Genomes" sheetId="2" r:id="rId2"/>
+    <sheet name="Gadiformes" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Gadiformes!$A$1:$A$10</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="225">
   <si>
     <t>Species</t>
   </si>
@@ -316,12 +321,6 @@
     <t>Chaenocephalus aceratus</t>
   </si>
   <si>
-    <t>SRR6942631</t>
-  </si>
-  <si>
-    <t>SRR6942632</t>
-  </si>
-  <si>
     <t>SRR6929341</t>
   </si>
   <si>
@@ -518,13 +517,202 @@
   </si>
   <si>
     <t>SRR3133083</t>
+  </si>
+  <si>
+    <t>Parablennius parvicornis</t>
+  </si>
+  <si>
+    <t>Thunnus albacares</t>
+  </si>
+  <si>
+    <t>Acanthochaenus luetkenii</t>
+  </si>
+  <si>
+    <t>Holocentrus rufus</t>
+  </si>
+  <si>
+    <t>Gadus morhua</t>
+  </si>
+  <si>
+    <t>Lota lota</t>
+  </si>
+  <si>
+    <t>Macrourus berglax</t>
+  </si>
+  <si>
+    <t>Muraenolepis marmoratus</t>
+  </si>
+  <si>
+    <t>Cyttopsis rosea</t>
+  </si>
+  <si>
+    <t>Borostomias antarcticus</t>
+  </si>
+  <si>
+    <t>Cottoperca gobio</t>
+  </si>
+  <si>
+    <t>ASM90030232v1</t>
+  </si>
+  <si>
+    <t>ASM90030235v1</t>
+  </si>
+  <si>
+    <t>ASM90030236v1</t>
+  </si>
+  <si>
+    <t>ASM90030238v1</t>
+  </si>
+  <si>
+    <t>ASM90030261v1</t>
+  </si>
+  <si>
+    <t>ASM90030262v1</t>
+  </si>
+  <si>
+    <t>ASM90030274v1</t>
+  </si>
+  <si>
+    <t>ASM90030267v1</t>
+  </si>
+  <si>
+    <t>ASM90031257v1</t>
+  </si>
+  <si>
+    <t>ASM90032332v1</t>
+  </si>
+  <si>
+    <t>ASM90030256v1</t>
+  </si>
+  <si>
+    <t>ERR2587161_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587161_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587165_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587165_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587193_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587193_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR2823736_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR2823736_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR3342841_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR3342841_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR4279902_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR4279902_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR5210463_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR5210463_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR5210464_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR5210464_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6793935_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6793935_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6794062_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6794062_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6929342_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6929342_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR7164558_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR7164558_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6450838_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR6450838_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR793598_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR793598_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587158_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>ERR2587158_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR8767971_1.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>SRR8767971_2.overep_filtered.fq</t>
+  </si>
+  <si>
+    <t>sculpin genome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perca </t>
+  </si>
+  <si>
+    <t>shallow rockfish</t>
+  </si>
+  <si>
+    <t>stickleback</t>
+  </si>
+  <si>
+    <t>grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">danio </t>
+  </si>
+  <si>
+    <t>pick other teleosts used in that cod paper</t>
+  </si>
+  <si>
+    <t>poly-igrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all these other genes have </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +731,25 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -568,10 +775,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CD3FE1-C10C-4CC2-9B17-9BF4EF33D9D6}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1267,7 @@
       <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1264,7 +1481,7 @@
       <c r="C27" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1275,7 +1492,7 @@
       <c r="C28" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1286,7 +1503,7 @@
       <c r="C29" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1297,7 +1514,7 @@
       <c r="C30" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1308,7 +1525,7 @@
       <c r="C31" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1319,7 +1536,7 @@
       <c r="C32" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1330,7 +1547,7 @@
       <c r="C33" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1341,7 +1558,7 @@
       <c r="C34" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1352,7 +1569,7 @@
       <c r="C35" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1363,7 +1580,7 @@
       <c r="C36" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1374,7 +1591,7 @@
       <c r="C37" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1385,7 +1602,7 @@
       <c r="C38" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1396,7 +1613,7 @@
       <c r="C39" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1407,7 +1624,7 @@
       <c r="C40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1418,7 +1635,7 @@
       <c r="C41" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1429,7 +1646,7 @@
       <c r="C42" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1440,7 +1657,7 @@
       <c r="C43" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="3" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1451,7 +1668,7 @@
       <c r="C44" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1462,7 +1679,7 @@
       <c r="C45" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1473,7 +1690,7 @@
       <c r="C46" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1484,7 +1701,7 @@
       <c r="C47" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="3" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1495,7 +1712,7 @@
       <c r="C48" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="3" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1506,8 +1723,8 @@
       <c r="C49" t="s">
         <v>50</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>98</v>
+      <c r="E49" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,10 +1732,10 @@
         <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,8 +1745,8 @@
       <c r="C51" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>101</v>
+      <c r="E51" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,8 +1756,8 @@
       <c r="C52" t="s">
         <v>57</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>102</v>
+      <c r="E52" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1550,8 +1767,8 @@
       <c r="C53" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>103</v>
+      <c r="E53" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1559,395 +1776,397 @@
         <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
         <v>57</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>107</v>
+      <c r="E55" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C56" t="s">
-        <v>109</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
         <v>67</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>113</v>
+      <c r="E59" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C60" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>114</v>
+      <c r="E60" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" t="s">
+        <v>114</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C61" t="s">
-        <v>116</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" t="s">
         <v>118</v>
       </c>
-      <c r="C62" t="s">
-        <v>120</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>119</v>
+      <c r="E62" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>121</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" t="s">
+        <v>119</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="C65" t="s">
-        <v>121</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C66" t="s">
-        <v>127</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C67" t="s">
-        <v>130</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" t="s">
         <v>129</v>
       </c>
-      <c r="C68" t="s">
-        <v>131</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>134</v>
+      <c r="E68" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C70" t="s">
-        <v>161</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C71" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C72" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>137</v>
+      <c r="E72" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C73" t="s">
         <v>57</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>136</v>
-      </c>
-      <c r="C74" t="s">
-        <v>140</v>
-      </c>
+      <c r="D74" s="2"/>
       <c r="E74" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C75" t="s">
+        <v>138</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" t="s">
+        <v>142</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="C76" t="s">
-        <v>144</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C77" t="s">
+        <v>142</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C78" t="s">
-        <v>147</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
+        <v>145</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C80" t="s">
-        <v>147</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C81" t="s">
-        <v>147</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C82" t="s">
-        <v>147</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>147</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C84" t="s">
         <v>67</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>155</v>
+      <c r="E84" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C85" t="s">
         <v>69</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>156</v>
+      <c r="E85" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C86" t="s">
         <v>57</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>157</v>
+      <c r="E86" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C87" t="s">
-        <v>100</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>158</v>
+        <v>98</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>159</v>
+        <v>107</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C89" t="s">
         <v>62</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>160</v>
+      <c r="E89" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1958,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C51996-481A-479D-8EB4-5B73A655493A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,24 +2192,435 @@
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>106</v>
-      </c>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F5A09C-A725-488B-9FF0-62A73C3F36DB}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F4FD77-DBAE-4C6D-8435-6C9853C21E16}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B32">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>